<commit_message>
perform export excel file
</commit_message>
<xml_diff>
--- a/Java_QuanLySinhVien/student_sheet.xlsx
+++ b/Java_QuanLySinhVien/student_sheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="93">
   <si>
     <t>Mã sinh viên</t>
   </si>
@@ -47,163 +47,166 @@
     <t>01/01/2004</t>
   </si>
   <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>Kế toán 5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin 1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>30/04/2000</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>Kiểm toán 1</t>
+  </si>
+  <si>
+    <t>Hà Nam</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn X</t>
+  </si>
+  <si>
+    <t>05/05/2005</t>
+  </si>
+  <si>
+    <t>test tiếp</t>
+  </si>
+  <si>
+    <t>Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>2022579490</t>
+  </si>
+  <si>
+    <t>Ngô Sỹ Anh</t>
+  </si>
+  <si>
+    <t>10/12/2001</t>
+  </si>
+  <si>
+    <t>Kế toán 1</t>
+  </si>
+  <si>
+    <t>Nghệ An</t>
+  </si>
+  <si>
+    <t>2020605565</t>
+  </si>
+  <si>
+    <t>Vũ Mạnh Dũng</t>
+  </si>
+  <si>
+    <t>11/12/2002</t>
+  </si>
+  <si>
+    <t>3.18</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin 4</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>nguyễn văn a</t>
+  </si>
+  <si>
+    <t>21/1/2000</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phầm mềm 2</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>nguyễn văn b</t>
+  </si>
+  <si>
+    <t>Cơ khí 2</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>nguyễn văn c</t>
+  </si>
+  <si>
+    <t>21/01/2000</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Quản trị kinh doanh 2</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>2022759455</t>
+  </si>
+  <si>
+    <t>22/12/2004</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>test nào</t>
+  </si>
+  <si>
+    <t>12/02/2002</t>
+  </si>
+  <si>
     <t>1.0</t>
-  </si>
-  <si>
-    <t>Kế toán 5</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin 1</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>30/04/2000</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>Kiểm toán 1</t>
-  </si>
-  <si>
-    <t>Hà Nam</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn X</t>
-  </si>
-  <si>
-    <t>05/05/2005</t>
-  </si>
-  <si>
-    <t>test tiếp</t>
-  </si>
-  <si>
-    <t>Vĩnh Phúc</t>
-  </si>
-  <si>
-    <t>2022579490</t>
-  </si>
-  <si>
-    <t>Ngô Sỹ Anh</t>
-  </si>
-  <si>
-    <t>10/12/2001</t>
-  </si>
-  <si>
-    <t>Kế toán 1</t>
-  </si>
-  <si>
-    <t>Nghệ An</t>
-  </si>
-  <si>
-    <t>2020605565</t>
-  </si>
-  <si>
-    <t>Vũ Mạnh Dũng</t>
-  </si>
-  <si>
-    <t>11/12/2002</t>
-  </si>
-  <si>
-    <t>3.18</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin 4</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>nguyễn văn a</t>
-  </si>
-  <si>
-    <t>21/1/2000</t>
-  </si>
-  <si>
-    <t>2.6</t>
-  </si>
-  <si>
-    <t>Kỹ thuật phầm mềm 2</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>nguyễn văn b</t>
-  </si>
-  <si>
-    <t>Cơ khí 2</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>nguyễn văn c</t>
-  </si>
-  <si>
-    <t>Kế toán 4</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>Quản trị kinh doanh 2</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>2022759455</t>
-  </si>
-  <si>
-    <t>22/12/2004</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>test nào</t>
-  </si>
-  <si>
-    <t>12/02/2002</t>
   </si>
   <si>
     <t>2021317801</t>
@@ -648,13 +651,13 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
         <v>39</v>
@@ -743,7 +746,7 @@
         <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -754,39 +757,39 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
@@ -795,71 +798,71 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21"/>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>74</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G23" t="s">
         <v>39</v>
@@ -867,19 +870,19 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -890,22 +893,22 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G25" t="s">
         <v>28</v>
@@ -913,16 +916,16 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
         <v>41</v>
@@ -931,7 +934,7 @@
         <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>